<commit_message>
Fix date consistency and template description per review feedback
Co-authored-by: VoxForgeHQ <255733893+VoxForgeHQ@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/workbooks/Excel-Copilot-Demo-Pack.xlsx
+++ b/workbooks/Excel-Copilot-Demo-Pack.xlsx
@@ -1661,7 +1661,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1693,7 +1693,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Pending</t>
+          <t>Completed</t>
         </is>
       </c>
     </row>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2026-04-15</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2026-03-30</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-03-10</t>
+          <t>2026-03-10</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -2272,7 +2272,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-05-20</t>
+          <t>2026-05-20</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2026-04-05</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -2376,7 +2376,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2026-03-25</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-03-15</t>
+          <t>2026-03-15</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-04-18</t>
+          <t>2026-04-18</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-05-30</t>
+          <t>2026-05-30</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-03-28</t>
+          <t>2026-03-28</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -2688,7 +2688,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2026-04-12</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-03-08</t>
+          <t>2026-03-08</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -2844,7 +2844,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-05-15</t>
+          <t>2026-05-15</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -2896,7 +2896,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-04-02</t>
+          <t>2026-04-02</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2948,7 +2948,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2026-04-08</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -3000,7 +3000,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-03-12</t>
+          <t>2026-03-12</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -3104,7 +3104,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-06-01</t>
+          <t>2026-06-01</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -3156,7 +3156,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-04-20</t>
+          <t>2026-04-20</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -3208,7 +3208,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2026-03-22</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2026-03-18</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -3312,7 +3312,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2026-04-10</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -3364,7 +3364,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-05-25</t>
+          <t>2026-05-25</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2026-03-27</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2026-04-15</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -3572,7 +3572,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2026-03-20</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -3709,12 +3709,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2026-03-31</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -3833,12 +3833,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2025-01-10</t>
+          <t>2026-01-10</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-03-30</t>
+          <t>2026-03-30</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3895,12 +3895,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2025-02-01</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-04-30</t>
+          <t>2026-04-30</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3957,12 +3957,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2025-02-15</t>
+          <t>2026-02-15</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-03-15</t>
+          <t>2026-03-15</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -4019,12 +4019,12 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2025-01-01</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-12-31</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -4143,12 +4143,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2025-02-01</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>2025-05-31</t>
+          <t>2026-05-31</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -4205,12 +4205,12 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2025-01-20</t>
+          <t>2026-01-20</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>2025-04-20</t>
+          <t>2026-04-20</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -4329,12 +4329,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2025-05-31</t>
+          <t>2026-05-31</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -4453,12 +4453,12 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2025-02-20</t>
+          <t>2026-02-20</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2025-04-30</t>
+          <t>2026-04-30</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -4515,12 +4515,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2025-01-05</t>
+          <t>2026-01-05</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>2025-06-30</t>
+          <t>2026-06-30</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -4577,12 +4577,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2025-02-01</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2026-03-31</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4701,12 +4701,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>2025-05-31</t>
+          <t>2026-05-31</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -4763,12 +4763,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2025-04-15</t>
+          <t>2026-04-15</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>2025-04-17</t>
+          <t>2026-04-17</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -4825,12 +4825,12 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2025-01-01</t>
+          <t>2026-01-01</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>2025-12-31</t>
+          <t>2026-12-31</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -4949,12 +4949,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2025-03-10</t>
+          <t>2026-03-10</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2026-04-10</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -5073,12 +5073,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2025-02-01</t>
+          <t>2026-02-01</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>2025-03-31</t>
+          <t>2026-03-31</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -5197,12 +5197,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2025-04-30</t>
+          <t>2026-04-30</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -6046,7 +6046,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -6108,7 +6108,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-03-01</t>
+          <t>2026-03-01</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -6170,7 +6170,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-03-05</t>
+          <t>2026-03-05</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -6232,7 +6232,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-03-08</t>
+          <t>2026-03-08</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -6294,7 +6294,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-03-10</t>
+          <t>2026-03-10</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -6356,7 +6356,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-03-12</t>
+          <t>2026-03-12</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -6418,7 +6418,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-03-15</t>
+          <t>2026-03-15</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -6480,7 +6480,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-03-15</t>
+          <t>2026-03-15</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -6542,7 +6542,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-03-18</t>
+          <t>2026-03-18</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -6604,7 +6604,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-03-20</t>
+          <t>2026-03-20</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -6666,7 +6666,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-03-22</t>
+          <t>2026-03-22</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -6728,7 +6728,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2026-03-25</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -6790,7 +6790,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-03-27</t>
+          <t>2026-03-27</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -6852,7 +6852,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-04-01</t>
+          <t>2026-04-01</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -6914,7 +6914,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-04-03</t>
+          <t>2026-04-03</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -6976,7 +6976,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-04-05</t>
+          <t>2026-04-05</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-04-08</t>
+          <t>2026-04-08</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -7100,7 +7100,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-04-10</t>
+          <t>2026-04-10</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -7162,7 +7162,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-04-12</t>
+          <t>2026-04-12</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">

</xml_diff>